<commit_message>
added excel read options
</commit_message>
<xml_diff>
--- a/Deepesh/PythonProgramming/Python_FileHandling/users_data.xlsx
+++ b/Deepesh/PythonProgramming/Python_FileHandling/users_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trainings\GTM_PS_Batch14_7Nov25\GTM_PS_BATCH14\Deepesh\PythonProgramming\Python_FileHandling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1535F234-BB93-4416-9B06-ADAF3CCDF411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A5E44F-6766-43E3-A55C-72EAA12DA377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="96">
   <si>
     <t>Pune1</t>
   </si>
@@ -260,13 +260,64 @@
   </si>
   <si>
     <t>pass4</t>
+  </si>
+  <si>
+    <t>user1@gmail.com</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>user5</t>
+  </si>
+  <si>
+    <t>pass5</t>
+  </si>
+  <si>
+    <t>user6</t>
+  </si>
+  <si>
+    <t>pass6</t>
+  </si>
+  <si>
+    <t>user7</t>
+  </si>
+  <si>
+    <t>pass7</t>
+  </si>
+  <si>
+    <t>user8</t>
+  </si>
+  <si>
+    <t>pass8</t>
+  </si>
+  <si>
+    <t>user9</t>
+  </si>
+  <si>
+    <t>pass9</t>
+  </si>
+  <si>
+    <t>user10</t>
+  </si>
+  <si>
+    <t>pass10</t>
+  </si>
+  <si>
+    <t>user11</t>
+  </si>
+  <si>
+    <t>pass11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +327,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -298,13 +357,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -585,12 +647,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1454,53 +1517,199 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>69</v>
       </c>
       <c r="B1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2">
+        <v>7870897987</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3">
+        <v>7870897987</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4">
+        <v>7870897987</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>78</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5">
+        <v>7870897987</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6">
+        <v>7870897988</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7">
+        <v>7870897989</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8">
+        <v>7870897990</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9">
+        <v>7870897991</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10">
+        <v>7870897992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11">
+        <v>7870897993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12">
+        <v>7870897994</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{92386643-8895-4EC9-88F7-C2A0D6403BA1}"/>
+    <hyperlink ref="C3:C5" r:id="rId2" display="user1@gmail.com" xr:uid="{D1DD0CB4-AB37-49CA-B733-1597514D4F52}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{0BBEB8F3-F026-4E07-91A7-8EF6CAA55317}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{5658FCC9-F621-474E-AA95-6F30873650C9}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{1F5F9565-61A6-4FD0-BC23-D05CF750C2CD}"/>
+    <hyperlink ref="C9" r:id="rId6" xr:uid="{290A401E-7093-4D3A-AAD0-309BF0F30735}"/>
+    <hyperlink ref="C10" r:id="rId7" xr:uid="{7AAECB2C-73FC-4999-B9F9-573D6B76BA20}"/>
+    <hyperlink ref="C11" r:id="rId8" xr:uid="{3F7ECCB7-E75B-4604-89EB-9305E57C6385}"/>
+    <hyperlink ref="C12" r:id="rId9" xr:uid="{F82A1196-C5B9-45C9-B5B9-53ECB2D90DAA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>